<commit_message>
Dynamic execution logic and validations
</commit_message>
<xml_diff>
--- a/testData/Test_Data.xlsx
+++ b/testData/Test_Data.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vrush\Automation\PythonAutomation\PostgreSQL\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vrush\Automation\PythonAutomation\PostgreSQL_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7114C90-647E-4D34-B31A-17D3C33B2F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F0614E-F993-4269-91B8-6A8837AAD45E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB_Connection" sheetId="2" r:id="rId1"/>
     <sheet name="TestData" sheetId="3" r:id="rId2"/>
+    <sheet name="DynamicTestData" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Sr No</t>
   </si>
@@ -65,17 +66,89 @@
     <t>SELECT version();</t>
   </si>
   <si>
-    <t>select * from get_dest_prediction('72e18c9e-0a2e-ff7e-bc63-d7348b8caec8', cast('2019-12-19 08:10:00-08' as timestamptz)) order by score desc;</t>
-  </si>
-  <si>
-    <t>Shopping</t>
+    <t>select distinct cc.usertableid
+        ,ST_GeoHash(ST_SetSRID(cast(cc.centroid as geometry), 4326), 6) as geohash
+        ,tz.tzid
+        ,get_srid_utmzone(cast(cc.centroid as geometry)) AS srid
+FROM cluster_centroid cc
+JOIN tz_world.tz_world tz on ST_Contains(tz.geom, CAST(cc.centroid as geometry))
+order by cc.usertableid, geohash;</t>
+  </si>
+  <si>
+    <t>select count(1) as cnt
+from (
+SELECT idt.usertableid
+        ,cm.centroidid
+        ,ST_Y(cast(geo.loc as geometry)) || ', ' || ST_X(cast(geo.loc as geometry)) as latlng
+        ,geo.idtableid
+        ,(lag(geo.idtableid) OVER (ORDER BY geo.timestampin)) as prev_idtableid
+        ,ct.name as assigned_label
+        ,ST_Distance(geo.loc, lag(geo.loc) OVER (ORDER BY geo.timestampin)) as distance
+        ,cast(
+                 (lag(et.eventname) OVER (ORDER BY geo.timestampin)) is null
+                 or
+                 (
+                        (et.eventname = 'powerOn' and (lag(et.eventname) OVER (ORDER BY geo.timestampin)) = 'powerOff')
+                         and
+                         ST_Distance(geo.loc, lag(geo.loc) OVER (ORDER BY geo.timestampin)) &lt; 300
+                 )
+                 or
+                 (
+                        (et.eventname = 'powerOff' and (lag(et.eventname) OVER (ORDER BY geo.timestampin)) = 'powerOn')
+                        and
+                        (geo.idtableid = (lag(geo.idtableid) OVER (ORDER BY geo.timestampin)))
+                 )
+         as int) as is_matched
+        ,et.eventname
+        ,(lag(et.eventname) OVER (ORDER BY geo.timestampin)) as prev_eventname
+FROM eventtable ev
+LEFT JOIN geolocation geo on ev.geolocationid = geo.id
+LEFT JOIN idtable idt on idt.id = geo.idtableid LEFT JOIN cluster_mapping cm on cm.eventid = ev.id
+LEFT JOIN eventtype et on ev.eventtypeid = et.id
+LEFT JOIN cluster_centroid cc on cc.id = cm.centroidid
+LEFT JOIN category ct on cc.categoryid = ct.id
+WHERE idt.usertableid = 54 AND et.eventname IN ('powerOn', 'powerOff')
+)
+aa
+where aa.is_matched = 0
+;</t>
+  </si>
+  <si>
+    <t>Sr.No</t>
+  </si>
+  <si>
+    <t>60bf53bb-c716-abcb-b079-45da4b6c421b</t>
+  </si>
+  <si>
+    <t>72e18c9e-0a2e-ff7e-bc63-d7348b8caec8</t>
+  </si>
+  <si>
+    <t>dbc8613a-d84c-5e60-f641-1030c66493f0</t>
+  </si>
+  <si>
+    <t>5c5dca5f-1b98-fff9-f111-8072b41c5fb3</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>select usertableid, start_label, end_label, score_rank from get_route_prediction('userId', '2020-01-31 15:15:16+00')</t>
+  </si>
+  <si>
+    <t>select * from public.get_preferred_media('userId', cast('2020-01-31 08:15:00-08' as timestamptz)) order by media_count desc;</t>
+  </si>
+  <si>
+    <t>select * from get_dest_prediction('userId', cast('2020-01-31 08:10:00-08' as timestamptz)) order by score desc;</t>
+  </si>
+  <si>
+    <t>select * from get_dest_prediction('userId', cast('2019-12-19 08:10:00-08' as timestamptz)) order by score desc;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +163,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -133,12 +212,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B51595-B499-4416-9792-8177212A957B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -508,22 +599,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91232A1-9384-411F-BB84-47E160174246}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.90625" customWidth="1"/>
+    <col min="2" max="2" width="89.6328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -537,22 +628,119 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CE00CA-1C92-42D5-B24E-19F80EE2D380}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="35.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>